<commit_message>
Added The_Child_Autism_Spectrum_Quotient_Questionnaire and cleaned up CBQ Excel File
</commit_message>
<xml_diff>
--- a/Quizzes/Childrens_Behavior_Questionnaire.xlsx
+++ b/Quizzes/Childrens_Behavior_Questionnaire.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagunkarki/Desktop/survey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickkleinsasser/Documents/Survey-App/Quizzes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59119E2C-7EA5-3C4E-9326-C8BA8334DB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44327AEC-8E48-A042-8B37-F3B9F6B11E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
-    <sheet name="result" sheetId="3" r:id="rId2"/>
-    <sheet name="abbrevations" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="217">
   <si>
     <t>cbq_num</t>
   </si>
@@ -52,9 +50,6 @@
     <t>cbq_scale_cat</t>
   </si>
   <si>
-    <t>cbq_a</t>
-  </si>
-  <si>
     <t>Seems always in a big hurry to get from one place to another.</t>
   </si>
   <si>
@@ -692,19 +687,13 @@
   </si>
   <si>
     <t>Has a hard time concentrating on an activity when there are distracting noises.</t>
-  </si>
-  <si>
-    <t>short_form</t>
-  </si>
-  <si>
-    <t>full_form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,20 +706,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -753,85 +728,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Cambria"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -867,25 +773,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA3E91C3-6560-DE4F-9CCE-8DC26C8F0D5C}" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E1048576" xr:uid="{AA3E91C3-6560-DE4F-9CCE-8DC26C8F0D5C}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA3E91C3-6560-DE4F-9CCE-8DC26C8F0D5C}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D1048576" xr:uid="{AA3E91C3-6560-DE4F-9CCE-8DC26C8F0D5C}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{90FD4D4D-D914-7341-99EB-FB612C5F6CB1}" name="cbq_num"/>
     <tableColumn id="2" xr3:uid="{EF0657E0-2D72-7F42-A396-279134658CB9}" name="cbq_q"/>
     <tableColumn id="3" xr3:uid="{5DB1FA53-2534-0748-9B39-93163A1A8CDB}" name="reverse"/>
     <tableColumn id="4" xr3:uid="{A68F5495-04A7-5B4D-9290-3994AAB25A5D}" name="cbq_scale_cat"/>
-    <tableColumn id="5" xr3:uid="{F909D316-447C-3642-B5C4-27A63B3F06E7}" name="cbq_a"/>
-  </tableColumns>
-  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC43ED70-553B-1349-951D-A776EA76960F}" name="Table5" displayName="Table5" ref="A1:B1048576" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B1048576" xr:uid="{DC43ED70-553B-1349-951D-A776EA76960F}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F15319F8-8B3C-D742-884C-E7AB0F2941FE}" name="short_form" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{89F51AEF-EFD5-444A-910A-95247605FF9B}" name="full_form" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1176,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1084,7 @@
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1203,188 +1097,185 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,10 +1283,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
         <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1403,13 +1294,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1417,10 +1308,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1428,13 +1319,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1442,10 +1333,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1453,10 +1344,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1464,10 +1355,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1475,13 +1366,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1489,10 +1380,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,10 +1391,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,10 +1402,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1522,10 +1413,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1533,13 +1424,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1547,10 +1438,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1558,13 +1449,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1572,10 +1463,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1583,13 +1474,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1597,10 +1488,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1608,10 +1499,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1619,10 +1510,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1630,10 +1521,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1641,10 +1532,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,13 +1543,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,10 +1557,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1677,10 +1568,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1688,13 +1579,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1702,10 +1593,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1713,13 +1604,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1727,10 +1618,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1738,13 +1629,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1752,10 +1643,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1763,13 +1654,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1777,10 +1668,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,10 +1679,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1799,10 +1690,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1810,13 +1701,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1824,10 +1715,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1835,13 +1726,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,10 +1740,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1860,10 +1751,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1871,10 +1762,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1882,13 +1773,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1896,13 +1787,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1910,10 +1801,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1921,13 +1812,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1935,10 +1826,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1946,10 +1837,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1957,10 +1848,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1968,10 +1859,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1979,10 +1870,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1990,13 +1881,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2004,10 +1895,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2015,13 +1906,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2029,10 +1920,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2040,13 +1931,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2054,13 +1945,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2068,13 +1959,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2082,10 +1973,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2093,10 +1984,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2104,10 +1995,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2115,10 +2006,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2126,10 +2017,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2137,10 +2028,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2148,13 +2039,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2162,10 +2053,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2173,10 +2064,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2184,10 +2075,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D83" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2195,13 +2086,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2209,13 +2100,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2223,10 +2114,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2234,13 +2125,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2248,10 +2139,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2259,13 +2150,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2273,10 +2164,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2284,13 +2175,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,10 +2189,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D92" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2309,10 +2200,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2320,13 +2211,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D94" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2334,10 +2225,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D95" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2345,13 +2236,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2359,10 +2250,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D97" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2370,10 +2261,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2381,10 +2272,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2392,13 +2283,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D100" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2406,10 +2297,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2417,13 +2308,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" t="s">
         <v>14</v>
-      </c>
-      <c r="D102" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2431,13 +2322,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,10 +2336,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D104" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2456,10 +2347,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D105" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2467,10 +2358,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D106" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2478,10 +2369,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D107" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2489,10 +2380,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2500,13 +2391,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2514,13 +2405,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2528,10 +2419,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D111" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2539,13 +2430,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D112" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2553,13 +2444,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2567,10 +2458,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2578,10 +2469,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2589,10 +2480,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2600,10 +2491,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D117" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2611,10 +2502,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D118" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2622,10 +2513,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D119" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2633,13 +2524,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,13 +2538,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,13 +2552,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2675,13 +2566,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2689,13 +2580,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2703,10 +2594,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2714,10 +2605,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D126" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2725,13 +2616,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2739,10 +2630,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D128" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2750,10 +2641,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D129" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2761,13 +2652,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C130" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D130" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2775,10 +2666,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D131" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -2786,13 +2677,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D132" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2800,10 +2691,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D133" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2811,10 +2702,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D134" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2822,10 +2713,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D135" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -2833,13 +2724,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D136" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -2847,10 +2738,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D137" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -2858,13 +2749,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C138" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D138" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -2872,13 +2763,13 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C139" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -2886,10 +2777,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D140" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -2897,10 +2788,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D141" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,10 +2799,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -2919,13 +2810,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C143" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D143" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -2933,10 +2824,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -2944,10 +2835,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D145" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -2955,13 +2846,13 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D146" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -2969,10 +2860,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D147" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -2980,10 +2871,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D148" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -2991,10 +2882,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D149" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3002,13 +2893,13 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C150" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D150" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3016,13 +2907,13 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C151" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D151" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3030,10 +2921,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D152" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3041,10 +2932,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,10 +2943,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -3063,10 +2954,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D155" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -3074,10 +2965,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D156" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -3085,13 +2976,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C157" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D157" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3099,10 +2990,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D158" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -3110,13 +3001,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C159" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D159" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3124,13 +3015,13 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C160" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D160" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3138,10 +3029,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D161" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3149,13 +3040,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C162" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D162" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3163,13 +3054,13 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C163" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,10 +3068,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,10 +3079,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D165" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3199,13 +3090,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C166" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D166" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3213,10 +3104,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D167" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3224,13 +3115,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3238,10 +3129,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D169" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -3249,13 +3140,13 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C170" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D170" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3263,13 +3154,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C171" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D171" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3277,13 +3168,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C172" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D172" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3291,10 +3182,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D173" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3302,10 +3193,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D174" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3313,10 +3204,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D175" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3324,13 +3215,13 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C176" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D176" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -3338,13 +3229,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C177" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D177" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -3352,10 +3243,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D178" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -3363,10 +3254,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D179" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -3374,10 +3265,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D180" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -3385,10 +3276,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D181" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -3396,10 +3287,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D182" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -3407,10 +3298,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D183" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -3418,13 +3309,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D184" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -3432,13 +3323,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C185" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D185" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3446,10 +3337,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D186" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -3457,10 +3348,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D187" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -3468,10 +3359,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D188" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -3479,13 +3370,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D189" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -3493,10 +3384,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D190" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -3504,13 +3395,13 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C191" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" t="s">
         <v>14</v>
-      </c>
-      <c r="D191" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -3518,13 +3409,13 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C192" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -3532,13 +3423,13 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D193" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -3546,10 +3437,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D194" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -3557,10 +3448,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D195" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -3568,13 +3459,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C196" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D196" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3583,104 +3474,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA2C4AE-66F7-7241-9272-480D26122344}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7984BD27-6509-4349-8307-6D75B409016C}">
-  <dimension ref="A1:I19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>